<commit_message>
first push for engineers!
</commit_message>
<xml_diff>
--- a/Hours.xlsx
+++ b/Hours.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmann\Desktop\ShiftrCompletion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmann\Desktop\ShiftrCompletion\ShiftrCompletion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445E2E7E-3487-48FA-8228-4767EB6CBEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609DA0A7-09E5-46E6-913F-DA7B9F4CC72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{65AE49EA-0B44-44A4-9B62-BA04BA1691BB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Day of Week</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Total Hours</t>
   </si>
   <si>
-    <t>Ron</t>
-  </si>
-  <si>
-    <t>Shiftr Script</t>
-  </si>
-  <si>
     <t>Monday</t>
   </si>
   <si>
@@ -82,6 +76,9 @@
   </si>
   <si>
     <t>OH</t>
+  </si>
+  <si>
+    <t>Weekly Meeting</t>
   </si>
 </sst>
 </file>
@@ -205,9 +202,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -245,7 +242,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -351,7 +348,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -493,7 +490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -504,7 +501,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,10 +541,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>0.47916666666666669</v>
+        <v>0.5</v>
       </c>
       <c r="C2" s="1">
         <v>0.54166666666666663</v>
@@ -556,11 +553,11 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G2" s="4">
         <f>(C2-B2)*24</f>
-        <v>1.4999999999999987</v>
+        <v>0.99999999999999911</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>8</v>
@@ -568,102 +565,132 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
-        <v>0.5</v>
+        <v>0.5625</v>
       </c>
       <c r="C3" s="1">
-        <v>0.5625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G3" s="4">
-        <f>(C2-B2)*24</f>
-        <v>1.4999999999999987</v>
+        <f t="shared" ref="G3:G18" si="0">(C3-B3)*24</f>
+        <v>2.4999999999999991</v>
       </c>
       <c r="I3" s="8">
-        <f>SUM(G2:G8)</f>
-        <v>7.4999999999999973</v>
+        <f>SUM(G2:G10)</f>
+        <v>14.999999999999993</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>0.5</v>
+        <v>0.4375</v>
       </c>
       <c r="C4" s="1">
-        <v>0.5625</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G4" s="4">
-        <f>(C3-B3)*24</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>2.4999999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>0.5</v>
       </c>
       <c r="C5" s="1">
-        <v>0.5625</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" ref="G5:G13" si="0">(C5-B5)*24</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>2.4999999999999991</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
-        <v>0.5</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C6" s="1">
-        <v>0.5625</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G6" s="4">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1.4999999999999987</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.99999999999999911</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -698,37 +725,37 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G14" s="4">
-        <f t="shared" ref="G14:G30" si="1">(C14-B14)*24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G14:G30" si="1">(C19-B19)*24</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>